<commit_message>
commit TC Add 01-20
</commit_message>
<xml_diff>
--- a/UAT-Testcase-LeaveForm.xlsx
+++ b/UAT-Testcase-LeaveForm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CO-OP\CubeSoftTech_WorkingSpace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5852F907-CCD9-4BB2-A704-07DACDD6ECA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA7FF87-E256-4492-BB5B-E84DFF50D628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{CCCF8952-E977-4E69-B266-ED8C89073CA7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="381">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -2326,9 +2326,6 @@
   </si>
   <si>
     <t>Date : 01-07-2021 to 31-07-2021</t>
-  </si>
-  <si>
-    <t>Date : 01-01-2020 to 31-12-2020</t>
   </si>
   <si>
     <t>Date : 03-09-2021 to 03-09-2021</t>
@@ -3323,56 +3320,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t>1. พนักงานค้นหาคำร้องการลาโดยการระบุปีสำเร็จ สถานะไม่พบคำร้อง</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-    1.1  ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
-    1.2 ระบบแสดงข้อความในช่องกรอกวันที่ 01-01-2020 to 31-12-2020
-    1.3 ระบบแสดงข้อความในช่องกรอกวันที่ 01-01-2020 to 31-12-2020
-และระบบแสดงข้อมูลที่ตรงกับวันที่ที่ค้นหา 0 รายการ</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t>1. พนักงานค้นหาคำร้องการลาโดยการระบุปีสำเร็จ สถานะไม่พบคำร้อง</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-    1.1  ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
-    1.2 ระบบแสดงข้อความในช่องกรอกวันที่ 01-01-2020 to 31-12-2020
-    1.3 ระบบแสดงข้อความในช่องกรอกวันที่ 01-01-2021 to 31-12-2020
-และระบบแสดงข้อมูลที่ตรงกับวันที่ที่ค้นหา 0 รายการ</t>
-    </r>
-  </si>
-  <si>
     <t>ผู้ใช้ไต้องมีสัญญาณอินเตอร์เน็ต
 พนักงานต้องมีสิทธิ์ในการเข้าถึงฟังก์ชันการลา
 และเคยยื่นคำร้องการลาในระบบ
@@ -4676,68 +4623,6 @@
 The applicant : "test_it_role", Type of leave : "ลากิจ/ลาพักร้อน"
 Start date (Since) : 11-01-2022, End date (Until) : 12-01-2022
 Amount the day : 2.000, Status : "Waiting for approve"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t>1. พนักงานยื่นคำร้องการลาครึ่งวันสำเร็จ สถานะรออนุมัติ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-   1.1 ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
-   1.2 ระบบจะแสดงหน้าจอสำหรับกรอกข้อมูลการลา (LEAVE004)
-   1.3 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
-เป็นข้อมูลที่ผู้ใช้เลือก
-   1.4 ระบบจะแสดงหน้าจอปฏิทิน (LEAVE005) ของเดือนสิงหาคม ค.ศ. 2021
-   1.5 แสดงข้อมูลสำหรับข้อมูลการลา (LEAVE003) และแสดงข้อมูลในคอลัมน์ดังนี้
-Leave ID : เลขรหัสสำหรับการลา, Submit Date : วันและเวลา ณ ขณะที่ทำการทดสอบ
-The applicant : "test_it_role", Type of leave : "ลาอื่น ๆ"
-Start date (Since) : 03-09-2021, End date (Until) : 03-09-2021
-Amount the day : 1.000, Status : "Waiting for approve"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t>1. พนักงานยื่นคำร้องการลาครึ่งวันสำเร็จ สถานะรออนุมัติ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-   1.1 ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
-   1.2 ระบบจะแสดงหน้าจอสำหรับกรอกข้อมูลการลา (LEAVE004)
-   1.3 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
-เป็นข้อมูลที่ผู้ใช้เลือก
-   1.4 ระบบจะแสดงหน้าจอปฏิทิน (LEAVE005) ของเดือนสิงหาคม ค.ศ. 2021
-   1.5 แสดงข้อมูลสำหรับข้อมูลการลา (LEAVE003) และแสดงข้อมูลในคอลัมน์ดังนี้
-Leave ID : 3732, Submit Date : 26-08-2021 00:33
-The applicant : "test_it_role", Type of leave : "ลาอื่น ๆ"
-Start date (Since) : 03-09-2021, End date (Until) : 03-09-2021
-Amount the day : 1.000, Status : "Waiting for approve"</t>
     </r>
   </si>
   <si>
@@ -5211,15 +5096,6 @@
   </si>
   <si>
     <t>Type of leave : ลาอื่น ๆ
-Duration : 03-09-2021 to 03-09-2021
-Amount : 1
-Hours : 3
-half day leave : Morning
-Description : TC-LEAVE-EMP-019
-Reason : เป็นส่วนหนึ่งในการทดสอบ</t>
-  </si>
-  <si>
-    <t>Type of leave : ลาอื่น ๆ
 Duration : 03-09-2021 to 06-09-2021
 Amount : 2
 Hours : 2
@@ -5292,6 +5168,124 @@
 half day leave : -
 Description : TC-LEAVE-EMP-012
 Reason : เป็นส่วนหนึ่งในการทดสอบ</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">พนักงานยื่นคำร้องการลาในปีที่แล้วสำเร็จ สถานะรออนุมัติ
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Positive Case)</t>
+    </r>
+  </si>
+  <si>
+    <t>เป็นส่วนหนึ่งในการยื่นคำร้องการลา
+สามารถยื่นคำร้องการลาในปีก่อนหน้าได้</t>
+  </si>
+  <si>
+    <t>Type of leave : ลาอื่น ๆ
+Duration : 03-12-2020 to 03-12-2020
+Amount : 1
+Hours : -
+half day leave : -
+Description : TC-LEAVE-EMP-019
+Reason : เป็นส่วนหนึ่งในการทดสอบ</t>
+  </si>
+  <si>
+    <t>Date : 01-01-2019 to 31-12-2019</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t>1. พนักงานค้นหาคำร้องการลาโดยการระบุปีสำเร็จ สถานะไม่พบคำร้อง</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+    1.1  ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
+    1.2 ระบบแสดงข้อความในช่องกรอกวันที่ 01-01-2019 to 31-12-2019
+    1.3 ระบบแสดงข้อความในช่องกรอกวันที่ 01-01-2019 to 31-12-2019
+และระบบแสดงข้อมูลที่ตรงกับวันที่ที่ค้นหา 0 รายการ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t>1. พนักงานยื่นคำร้องการลาครึ่งวันสำเร็จ สถานะรออนุมัติ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+   1.1 ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
+   1.2 ระบบจะแสดงหน้าจอสำหรับกรอกข้อมูลการลา (LEAVE004)
+   1.3 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
+เป็นข้อมูลที่ผู้ใช้เลือก
+   1.4 ระบบจะแสดงหน้าจอปฏิทิน (LEAVE005) ของเดือนสิงหาคม ค.ศ. 2021
+   1.5 แสดงข้อมูลสำหรับข้อมูลการลา (LEAVE003) และแสดงข้อมูลในคอลัมน์ดังนี้
+Leave ID : เลขรหัสสำหรับการลา, Submit Date : วันและเวลา ณ ขณะที่ทำการทดสอบ
+The applicant : "test_it_role", Type of leave : "ลาอื่น ๆ"
+Start date (Since) :  03-12-2020, End date (Until) :  03-12-2020
+Amount the day : 1.000, Status : "Waiting for approve"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t>1. พนักงานยื่นคำร้องการลาครึ่งวันสำเร็จ สถานะรออนุมัติ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+   1.1 ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
+   1.2 ระบบจะแสดงหน้าจอสำหรับกรอกข้อมูลการลา (LEAVE004)
+   1.3 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
+เป็นข้อมูลที่ผู้ใช้เลือก
+   1.4 ระบบจะแสดงหน้าจอปฏิทิน (LEAVE005) ของเดือนสิงหาคม ค.ศ. 2021
+   1.5 แสดงข้อมูลสำหรับข้อมูลการลา (LEAVE003) และแสดงข้อมูลในคอลัมน์ดังนี้
+Leave ID : 3732, Submit Date : 26-08-2021 00:33
+The applicant : "test_it_role", Type of leave : "ลาอื่น ๆ"
+Start date (Since) :  03-12-2020, End date (Until) : 03-12-2020
+Amount the day : 1.000, Status : "Waiting for approve"</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -5452,7 +5446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5525,9 +5519,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7308,8 +7305,8 @@
   <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.6"/>
@@ -7327,14 +7324,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="30"/>
+      <c r="D1" s="31"/>
       <c r="E1" s="15" t="s">
         <v>10</v>
       </c>
@@ -7500,10 +7497,10 @@
         <v>43</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>18</v>
@@ -7531,10 +7528,10 @@
         <v>91</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I8" s="17" t="s">
         <v>183</v>
@@ -7566,10 +7563,10 @@
         <v>145</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="I9" s="18"/>
       <c r="J9" s="8"/>
@@ -7589,16 +7586,16 @@
         <v>138</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>146</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="I10" s="18"/>
       <c r="J10" s="8"/>
@@ -7618,16 +7615,16 @@
         <v>138</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>147</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="I11" s="18"/>
       <c r="J11" s="8"/>
@@ -7644,19 +7641,19 @@
         <v>34</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>196</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="I12" s="18"/>
       <c r="J12" s="8"/>
@@ -7676,16 +7673,16 @@
         <v>138</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>160</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I13" s="18"/>
       <c r="J13" s="8"/>
@@ -7705,16 +7702,16 @@
         <v>138</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>161</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="I14" s="18"/>
       <c r="J14" s="8"/>
@@ -7734,16 +7731,16 @@
         <v>138</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>162</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I15" s="16"/>
       <c r="J15" s="8" t="s">
@@ -7767,16 +7764,16 @@
         <v>138</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>163</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="I16" s="16"/>
       <c r="J16" s="8" t="s">
@@ -7800,7 +7797,7 @@
         <v>138</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>164</v>
@@ -7809,7 +7806,7 @@
         <v>189</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I17" s="16"/>
       <c r="J17" s="8" t="s">
@@ -7833,7 +7830,7 @@
         <v>138</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>165</v>
@@ -7842,7 +7839,7 @@
         <v>191</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I18" s="16"/>
       <c r="J18" s="8"/>
@@ -7864,16 +7861,16 @@
         <v>138</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>167</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I19" s="18"/>
       <c r="J19" s="8"/>
@@ -7895,13 +7892,13 @@
         <v>138</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>166</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>192</v>
@@ -7926,7 +7923,7 @@
         <v>138</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>208</v>
@@ -7957,16 +7954,16 @@
         <v>138</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>195</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I22" s="18"/>
       <c r="J22" s="8"/>
@@ -7977,25 +7974,25 @@
         <v>57</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>149</v>
+        <v>374</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>148</v>
+        <v>375</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>138</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>168</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>341</v>
+        <v>379</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>342</v>
+        <v>380</v>
       </c>
       <c r="I23" s="18"/>
       <c r="J23" s="8"/>
@@ -8015,16 +8012,16 @@
         <v>138</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>168</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="I24" s="18"/>
       <c r="J24" s="8"/>
@@ -8046,7 +8043,7 @@
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" s="10" customFormat="1" ht="273" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="32" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="13" t="s">
@@ -8065,10 +8062,10 @@
         <v>204</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="I26" s="18"/>
       <c r="J26" s="12"/>
@@ -8096,10 +8093,10 @@
         <v>205</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="I27" s="18"/>
       <c r="J27" s="12"/>
@@ -8109,7 +8106,7 @@
       <c r="A28" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="30" t="s">
         <v>75</v>
       </c>
       <c r="C28" s="13" t="s">
@@ -8125,10 +8122,10 @@
         <v>206</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I28" s="18"/>
       <c r="J28" s="12"/>
@@ -8138,7 +8135,7 @@
       <c r="A29" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="30" t="s">
         <v>76</v>
       </c>
       <c r="C29" s="13" t="s">
@@ -8154,10 +8151,10 @@
         <v>207</v>
       </c>
       <c r="G29" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="H29" s="7" t="s">
         <v>254</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>255</v>
       </c>
       <c r="I29" s="18"/>
       <c r="J29" s="12"/>
@@ -8167,14 +8164,14 @@
       <c r="A30" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="30" t="s">
         <v>154</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>122</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>158</v>
@@ -8183,10 +8180,10 @@
         <v>209</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="I30" s="18"/>
       <c r="J30" s="12"/>
@@ -8206,16 +8203,16 @@
         <v>143</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>211</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I31" s="18"/>
       <c r="J31" s="12" t="s">
@@ -8239,7 +8236,7 @@
         <v>143</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="F32" s="13" t="s">
         <v>210</v>
@@ -8248,7 +8245,7 @@
         <v>212</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I32" s="16"/>
       <c r="K32" s="12" t="s">
@@ -8269,16 +8266,16 @@
         <v>144</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>214</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="I33" s="18"/>
       <c r="J33" s="12" t="s">
@@ -8302,7 +8299,7 @@
         <v>144</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="F34" s="13" t="s">
         <v>216</v>
@@ -8344,7 +8341,7 @@
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K35" s="12" t="s">
         <v>220</v>
@@ -8411,13 +8408,13 @@
         <v>159</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I38" s="18"/>
       <c r="J38" s="12"/>
@@ -8440,13 +8437,13 @@
         <v>159</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I39" s="18"/>
       <c r="J39" s="12"/>
@@ -8469,13 +8466,13 @@
         <v>159</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I40" s="18"/>
       <c r="J40" s="12"/>
@@ -8492,19 +8489,19 @@
         <v>125</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="E41" s="12" t="s">
         <v>159</v>
       </c>
       <c r="F41" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="G41" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="G41" s="13" t="s">
-        <v>260</v>
-      </c>
       <c r="H41" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I41" s="18"/>
       <c r="J41" s="12"/>
@@ -8542,20 +8539,20 @@
         <v>228</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I43" s="16"/>
       <c r="J43" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="4" customFormat="1" ht="168" x14ac:dyDescent="0.3">
@@ -8572,23 +8569,23 @@
         <v>139</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I44" s="16"/>
       <c r="J44" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.3">
@@ -8608,20 +8605,20 @@
         <v>229</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G45" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="H45" s="7" t="s">
         <v>266</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>267</v>
       </c>
       <c r="I45" s="16"/>
       <c r="J45" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="409.6" x14ac:dyDescent="0.6">
@@ -8641,20 +8638,20 @@
         <v>230</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G46" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="H46" s="7" t="s">
         <v>268</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>269</v>
       </c>
       <c r="I46" s="16"/>
       <c r="J46" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="105" x14ac:dyDescent="0.6">
@@ -8674,20 +8671,20 @@
         <v>231</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H47" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I47" s="16"/>
       <c r="J47" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="168" x14ac:dyDescent="0.6">
@@ -8704,23 +8701,23 @@
         <v>139</v>
       </c>
       <c r="E48" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="G48" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="F48" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="G48" s="7" t="s">
+      <c r="H48" s="7" t="s">
         <v>273</v>
-      </c>
-      <c r="H48" s="7" t="s">
-        <v>274</v>
       </c>
       <c r="I48" s="16"/>
       <c r="J48" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="105" x14ac:dyDescent="0.6">
@@ -8737,23 +8734,23 @@
         <v>139</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>232</v>
+        <v>377</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>275</v>
+        <v>378</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>276</v>
+        <v>378</v>
       </c>
       <c r="I49" s="16"/>
       <c r="J49" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.6">
@@ -8782,26 +8779,26 @@
         <v>137</v>
       </c>
       <c r="D51" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="F51" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="G51" s="23" t="s">
         <v>277</v>
       </c>
-      <c r="E51" s="23" t="s">
-        <v>278</v>
-      </c>
-      <c r="F51" s="23" t="s">
-        <v>279</v>
-      </c>
-      <c r="G51" s="23" t="s">
-        <v>280</v>
-      </c>
       <c r="H51" s="23" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="I51" s="24"/>
       <c r="J51" s="8" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="273" x14ac:dyDescent="0.6">
@@ -8815,19 +8812,19 @@
         <v>137</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E52" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="F52" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="F52" s="23" t="s">
-        <v>281</v>
-      </c>
       <c r="G52" s="23" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H52" s="23" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="I52" s="25"/>
       <c r="J52" s="11"/>
@@ -8862,16 +8859,16 @@
         <v>179</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G54" s="20" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="H54" s="20" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="I54" s="18"/>
       <c r="J54" s="11"/>
@@ -8891,16 +8888,16 @@
         <v>179</v>
       </c>
       <c r="E55" s="14" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G55" s="20" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H55" s="20" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="I55" s="18"/>
       <c r="J55" s="11"/>
@@ -8914,29 +8911,29 @@
         <v>172</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D56" s="13" t="s">
         <v>179</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="G56" s="20" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="H56" s="20" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="I56" s="16"/>
       <c r="J56" s="8" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="K56" s="7" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="126" x14ac:dyDescent="0.6">
@@ -8953,23 +8950,23 @@
         <v>179</v>
       </c>
       <c r="E57" s="14" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G57" s="20" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="H57" s="20" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="I57" s="16"/>
       <c r="J57" s="8" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="K57" s="7" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="126" x14ac:dyDescent="0.6">
@@ -8986,23 +8983,23 @@
         <v>179</v>
       </c>
       <c r="E58" s="14" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G58" s="20" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H58" s="20" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="I58" s="16"/>
       <c r="J58" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="K58" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="84" x14ac:dyDescent="0.6">
@@ -9010,10 +9007,10 @@
         <v>120</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D59" s="13" t="s">
         <v>179</v>
@@ -9022,13 +9019,13 @@
         <v>159</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G59" s="20" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H59" s="20" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="I59" s="18"/>
       <c r="J59" s="8"/>
@@ -9036,7 +9033,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A60" s="5" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -9054,38 +9051,38 @@
         <v>121</v>
       </c>
       <c r="B61" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="F61" s="14" t="s">
         <v>315</v>
       </c>
-      <c r="C61" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="F61" s="14" t="s">
+      <c r="G61" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="G61" s="7" t="s">
-        <v>321</v>
-      </c>
       <c r="H61" s="7" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="I61" s="16"/>
       <c r="J61" s="8" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="K61" s="8" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="L61" s="4"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A62" s="6" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -9104,13 +9101,13 @@
         <v>126</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C63" s="27" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="D63" s="27" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E63" s="26"/>
       <c r="F63" s="26"/>
@@ -9272,14 +9269,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="30"/>
+      <c r="D1" s="31"/>
       <c r="E1" s="15" t="s">
         <v>10</v>
       </c>
@@ -9362,7 +9359,7 @@
         <v>42</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>20</v>
@@ -9393,7 +9390,7 @@
         <v>42</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Commit TC 21-31 Edit
</commit_message>
<xml_diff>
--- a/UAT-Testcase-LeaveForm.xlsx
+++ b/UAT-Testcase-LeaveForm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CO-OP\CubeSoftTech_WorkingSpace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA7FF87-E256-4492-BB5B-E84DFF50D628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A003CDB-F1E7-409C-A801-2A2776F0E499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{CCCF8952-E977-4E69-B266-ED8C89073CA7}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="HR,Admin Role" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="386">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1238,21 +1239,6 @@
 โดยยึดวันหยุดนักขัตฤกษ์ตามธนาคารแห่งประเทศไทย</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">พนักงานแก้ไขประเภทการลาครึ่งวันสำเร็จ สถานะรออนุมัติ
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF00B050"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Positive Case)</t>
-    </r>
-  </si>
-  <si>
     <t>Type of leave : ลาอื่น ๆ</t>
   </si>
   <si>
@@ -1260,9 +1246,6 @@
   </si>
   <si>
     <t>Reason : เป็นส่วนหนึ่งในการทดสอบ Edit</t>
-  </si>
-  <si>
-    <t>half day leave : Afternoon</t>
   </si>
   <si>
     <t>-</t>
@@ -2167,135 +2150,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t>1. พนักงานแก้ไขคำร้องการลาโดยการย้ายปุ่มสำเร็จ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-    1.1 กดปุ่ม Calendar
-    1.2 กดปุ่ม Check All Calendar
-    1.3 เลือก ลาอื่น ๆ ในวันที่ 20 สิงหาคม 2021 ย้ายไปที่ 19 สิงหาคม 2021
-    1.4 ทำการ refresh หน้าเพจ
-    1.5 กดปุ่ม My Leave และตรวจสอบข้อมูลของ Leave ID 3724</t>
-    </r>
-  </si>
-  <si>
     <t>ไม่สามารถย้ายข้อมูลการลาได้ในหน้าปฏิทิน</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t>1. พนักงานแก้ไขคำร้องการลาโดยการย้ายปุ่มไม่สำเร็จ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-    1.1 กดปุ่ม Calendar
-    1.2 กดปุ่ม Check All Calendar
-    1.3 เลือก ลาอื่น ๆ ในวันที่ 20 สิงหาคม 2021 ย้ายไปที่ 19 สิงหาคม 2021</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t>1. พนักงานแก้ไขคำร้องการลาโดยการย้ายปุ่มสำเร็จ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-    1.1 แสดงปุ่มย่อยให้เลือก (drop down)
-    1.2 ระบบแสดงหน้าจอ (LEAVE008) เพื่อแสดงข้อมูลทั้งหมดของผู้ใช้ 
-    1.3 ตัวเลือก ลาป่วย  ในวันที่ 20 สิงหาคม 2021 ไม่สามารถย้ายไปที่ 19 สิงหาคม 2021</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t>1. พนักงานแก้ไขคำร้องการลาโดยการย้ายปุ่มสำเร็จ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-    1.1 แสดงปุ่มย่อยให้เลือก (drop down)
-    1.2 ระบบแสดงหน้าจอ (LEAVE008) เพื่อแสดงข้อมูลทั้งหมดของผู้ใช้ 
-    1.3 ตัวเลือก ลาป่วย  ในวันที่ 20 สิงหาคม 2021 ย้ายไปที่ 19 สิงหาคม 2021
-    1.4 ข้อมูลการลาถูกย้ายไปยังวันที่ 3 สิงหาคม 2021
-    1.5 ระบบแสดงหน้าจอสำหรับข้อมูลการลา (LEAVE003) และข้อมูลมีการเปี่ยนแปลงดังนี้
-Leave ID : 3724, Submit Date : 25-08-2021 11:14
-The applicant : "test_it_role", Type of leave : "ลาป่วย"
-Start date (Since) : 19-08-2021, End date (Until) : 19-08-2021
-Amount the day : 1.000, Status : "Waiting for approve"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t>1. พนักงานแก้ไขคำร้องการลาโดยการย้ายปุ่มไม่สำเร็จ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-    1.1 แสดงปุ่มย่อยให้เลือก (drop down)
-    1.2 ระบบแสดงหน้าจอ (LEAVE008) เพื่อแสดงข้อมูลทั้งหมดของผู้ใช้ 
-    1.3 ตัวเลือก ลาป่วย  ในวันที่ 20 สิงหาคม 2021 ไม่สามารถย้ายไปที่ 19 สิงหาคม 2021 ได้</t>
-    </r>
   </si>
   <si>
     <t>ผู้ใช้ต้องมีสัญญาณอินเตอร์เน็ต
@@ -4634,68 +4489,6 @@
         <rFont val="TH Sarabun New"/>
         <family val="2"/>
       </rPr>
-      <t>1. พนักงานยื่นคำร้องการลาครึ่งวันสำเร็จ สถานะรออนุมัติ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-   1.1 ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
-   1.2 ระบบจะแสดงหน้าจอสำหรับกรอกข้อมูลการลา (LEAVE004)
-   1.3 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
-เป็นข้อมูลที่ผู้ใช้เลือก
-   1.4 ระบบจะแสดงหน้าจอปฏิทิน (LEAVE005) ของเดือนสิงหาคม ค.ศ. 2021
-   1.5 แสดงข้อมูลสำหรับข้อมูลการลา (LEAVE003) และแสดงข้อมูลในคอลัมน์ดังนี้
-Leave ID : เลขรหัสสำหรับการลา, Submit Date : วันและเวลา ณ ขณะที่ทำการทดสอบ
-The applicant : "test_it_role", Type of leave : "ลาอื่น ๆ"
-Start date (Since) : 03-09-2021, End date (Until) : 06-09-2021
-Amount the day : 2.000, Status : "Waiting for approve"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t>1. พนักงานยื่นคำร้องการลาครึ่งวันสำเร็จ สถานะรออนุมัติ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-   1.1 ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
-   1.2 ระบบจะแสดงหน้าจอสำหรับกรอกข้อมูลการลา (LEAVE004)
-   1.3 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
-เป็นข้อมูลที่ผู้ใช้เลือก
-   1.4 ระบบจะแสดงหน้าจอปฏิทิน (LEAVE005) ของเดือนสิงหาคม ค.ศ. 2021
-   1.5 แสดงข้อมูลสำหรับข้อมูลการลา (LEAVE003) และแสดงข้อมูลในคอลัมน์ดังนี้
-Leave ID : 3733, Submit Date : 26-08-2021 00:37
-The applicant : "test_it_role", Type of leave : "ลาอื่น ๆ"
-Start date (Since) : 03-09-2021, End date (Until) : 06-09-2021
-Amount the day : 2.000, Status : "Waiting for approve"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
       <t>1. พนักงานแก้ไขประเภทคำร้องการลาสำเร็จ สถานะรออนุมัติ</t>
     </r>
     <r>
@@ -4784,72 +4577,6 @@
 Amount the day : 1.000, Status : "Waiting for approve"
    1.6 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
 เป็นข้อมูลที่ผู้ใช้เลือก และคำอธิบายของการลาเปลี่ยนแปลงเป็น "TC-LEAVE-EMP-006 Edit"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t>พนักงานแก้ไขประเภทการลาครึ่งวันสำเร็จ สถานะรออนุมัติ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-   1.1 ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
-   1.2 ระบบจะแสดงหน้าจอสำหรับกรอกข้อมูลการลา (LEAVE004)
-   1.3 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
-เป็นข้อมูลที่ผู้ใช้เลือก
-   1.4 ระบบจะแสดงหน้าจอข้อมูลการลาทั้งหมด (LEAVE007) 
-   1.5 แสดงข้อมูลสำหรับข้อมูลการลา (LEAVE003) และแสดงข้อมูลในคอลัมน์ดังนี้
-Leave ID : 3732, Submit Date : 26-08-2021 00:33
-The applicant : "test_it_role", Type of leave : "ลาอื่นๆ"
-Start date (Since) : 03-09-2021, End date (Until) : 03-09-2021
-Amount the day : 1.000, Status : "Waiting for approve"
-   1.6 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
-เป็นข้อมูลที่ผู้ใช้เลือก และhalf of day leave ของการลาเปลี่ยนแปลงเป็น "Afternoon"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t>พนักงานแก้ไขประเภทการลาครึ่งวันสำเร็จ สถานะรออนุมัติ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="TH Sarabun New"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-   1.1 ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
-   1.2 ระบบจะแสดงหน้าจอสำหรับกรอกข้อมูลการลา (LEAVE004)
-   1.3 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
-เป็นข้อมูลที่ผู้ใช้เลือก
-   1.4 ระบบจะแสดงหน้าจอข้อมูลการลาทั้งหมด (LEAVE007) 
-   1.5 แสดงข้อมูลสำหรับข้อมูลการลา (LEAVE003) และแสดงข้อมูลในคอลัมน์ดังนี้
-Leave ID : 3732, Submit Date : 26-08-2021 00:33
-The applicant : "test_it_role", Type of leave : "ลาอื่น ๆ"
-Start date (Since) : 03-09-2021, End date (Until) : 03-09-2021
-Amount the day : 1.000, Status : "Waiting for approve"
-   1.6 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
-เป็นข้อมูลที่ผู้ใช้เลือก และhalf of day leave ของการลาเปลี่ยนแปลงเป็น "Afternoon"</t>
     </r>
   </si>
   <si>
@@ -5095,15 +4822,6 @@
 Reason : เป็นส่วนหนึ่งในการทดสอบ</t>
   </si>
   <si>
-    <t>Type of leave : ลาอื่น ๆ
-Duration : 03-09-2021 to 06-09-2021
-Amount : 2
-Hours : 2
-half day leave : Afternoon
-Description : TC-LEAVE-EMP-020
-Reason : เป็นส่วนหนึ่งในการทดสอบ</t>
-  </si>
-  <si>
     <t>Type of leave : ลาป่วย
 Description : , TC-LEAVE-EMP-026</t>
   </si>
@@ -5149,10 +4867,6 @@
 Hours : 0
 half day leave : -
 Description : TC-LEAVE-EMP-048</t>
-  </si>
-  <si>
-    <t>ผู้ใช้ไม่มีสัญญาณอินเตอร์เน็ต และต้องผ่านการทดสอบ
-ในเทสต์เคส TC-LEAVE-EMP-019</t>
   </si>
   <si>
     <t>ผู้ใช้ต้องมีสัญญาณอินเตอร์เน็ต
@@ -5285,6 +4999,360 @@
 The applicant : "test_it_role", Type of leave : "ลาอื่น ๆ"
 Start date (Since) :  03-12-2020, End date (Until) : 03-12-2020
 Amount the day : 1.000, Status : "Waiting for approve"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">พนักงานแก้ไขประเภทการลาครึ่งวันและชั่วโมงสำเร็จ สถานะรออนุมัติ
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Positive Case)</t>
+    </r>
+  </si>
+  <si>
+    <t>half day leave : Afternoon
+hours : 5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t>1. พนักงานยื่นคำร้องการลาครึ่งวันสำเร็จ สถานะรออนุมัติ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+   1.1 ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
+   1.2 ระบบจะแสดงหน้าจอสำหรับกรอกข้อมูลการลา (LEAVE004)
+   1.3 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
+เป็นข้อมูลที่ผู้ใช้เลือก
+   1.4 ระบบจะแสดงหน้าจอปฏิทิน (LEAVE005) ของเดือนสิงหาคม ค.ศ. 2021
+   1.5 แสดงข้อมูลสำหรับข้อมูลการลา (LEAVE003) และแสดงข้อมูลในคอลัมน์ดังนี้
+Leave ID : เลขรหัสสำหรับการลา, Submit Date : วันและเวลา ณ ขณะที่ทำการทดสอบ
+The applicant : "test_it_role", Type of leave : "ลาอื่น ๆ"
+Start date (Since) : 03-09-2021, End date (Until) : 06-09-2021
+Amount the day : 2.375, Status : "Waiting for approve"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t>1. พนักงานยื่นคำร้องการลาครึ่งวันสำเร็จ สถานะรออนุมัติ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+   1.1 ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
+   1.2 ระบบจะแสดงหน้าจอสำหรับกรอกข้อมูลการลา (LEAVE004)
+   1.3 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
+เป็นข้อมูลที่ผู้ใช้เลือก
+   1.4 ระบบจะแสดงหน้าจอปฏิทิน (LEAVE005) ของเดือนสิงหาคม ค.ศ. 2021
+   1.5 แสดงข้อมูลสำหรับข้อมูลการลา (LEAVE003) และแสดงข้อมูลในคอลัมน์ดังนี้
+Leave ID : 3733, Submit Date : 26-08-2021 00:37
+The applicant : "test_it_role", Type of leave : "ลาอื่น ๆ"
+Start date (Since) : 03-09-2021, End date (Until) : 06-09-2021
+Amount the day : 2.375, Status : "Waiting for approve"</t>
+    </r>
+  </si>
+  <si>
+    <t>Type of leave : ลาอื่น ๆ
+Duration : 03-09-2021 to 06-09-2021
+Amount : 2
+Hours : 3
+half day leave : Afternoon
+Description : TC-LEAVE-EMP-020
+Reason : เป็นส่วนหนึ่งในการทดสอบ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t>พนักงานแก้ไขประเภทการลาครึ่งวันสำเร็จ สถานะรออนุมัติ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+   1.1 ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
+   1.2 ระบบจะแสดงหน้าจอสำหรับกรอกข้อมูลการลา (LEAVE004)
+   1.3 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
+เป็นข้อมูลที่ผู้ใช้เลือก
+   1.4 ระบบจะแสดงหน้าจอข้อมูลการลาทั้งหมด (LEAVE007) 
+   1.5 แสดงข้อมูลสำหรับข้อมูลการลา (LEAVE003) และแสดงข้อมูลในคอลัมน์ดังนี้
+Leave ID : 3732, Submit Date : 26-08-2021 00:33
+The applicant : "test_it_role", Type of leave : "ลาอื่นๆ"
+Start date (Since) : 03-09-2021, End date (Until) : 06-09-2021
+Amount the day : 2.625, Status : "Waiting for approve"
+   1.6 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
+เป็นข้อมูลที่ผู้ใช้เลือก และhalf of day leave ของการลาเปลี่ยนแปลงเป็น "Afternoon"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t>พนักงานแก้ไขประเภทการลาครึ่งวันสำเร็จ สถานะรออนุมัติ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+   1.1 ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
+   1.2 ระบบจะแสดงหน้าจอสำหรับกรอกข้อมูลการลา (LEAVE004)
+   1.3 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
+เป็นข้อมูลที่ผู้ใช้เลือก
+   1.4 ระบบจะแสดงหน้าจอข้อมูลการลาทั้งหมด (LEAVE007) 
+   1.5 แสดงข้อมูลสำหรับข้อมูลการลา (LEAVE003) และแสดงข้อมูลในคอลัมน์ดังนี้
+Leave ID : 3732, Submit Date : 26-08-2021 00:33
+The applicant : "test_it_role", Type of leave : "ลาอื่น ๆ"
+Start date (Since) : 03-09-2021, End date (Until) : 03-09-2021
+Amount the day : 2.625, Status : "Waiting for approve"
+   1.6 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
+เป็นข้อมูลที่ผู้ใช้เลือก และhalf of day leave ของการลาเปลี่ยนแปลงเป็น "Afternoon"</t>
+    </r>
+  </si>
+  <si>
+    <t>ผู้ใช้มีสัญญาณอินเตอร์เน็ต และต้องผ่านการทดสอบ
+ในเทสต์เคส TC-LEAVE-EMP-020</t>
+  </si>
+  <si>
+    <t>Function Name : การทดสอบฟังก์ชันการลา (Leave Form)</t>
+  </si>
+  <si>
+    <t>Function ID : UAT-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ผู้ใช้ต้องมีสัญญาณอินเตอร์เน็ต </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t>1. พนักงานแก้ไขคำร้องการลาโดยการย้ายปุ่มไม่สำเร็จ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+   1.1 กดปุ่ม My Leave
+   1.2 กดปุ่ม Add leave
+   1.3 กรอกข้อมูลตามที่ระบุใน Input Data
+   1.4 กดปุ่ม Submit
+    1.5 กดปุ่ม Calendar
+    1.6 กดปุ่ม Check All Calendar
+    1.7 กดปุ่มถัดไป 
+    1.8 และเลือกลากิจ/ลาพักร้อน ในวันที่ 7 กันยายน 2021 ย้ายไปที่ 8 กันยายน 2021
+    1.9 กดปุ่ม My Leave และตรวจสอบข้อมูลของ Leave ID 3724</t>
+    </r>
+  </si>
+  <si>
+    <t>Type of leave : ลากิจ/ลาพักร้อน
+Duration : 06-09-2021 to 06-09-2021</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1. พนักงานแก้ไขคำร้องการลาโดยการย้ายปุ่มสำเร็จ
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   1.1 กดปุ่ม My Leave
+   1.2 กดปุ่ม Add leave
+   1.3 กรอกข้อมูลตามที่ระบุใน Input Data
+   1.4 กดปุ่ม Submit
+    1.5 กดปุ่ม Calendar
+    1.6 กดปุ่ม Check All Calendar
+    1.7 กดปุ่มถัดไป 
+    1.8 และเลือกลากิจ/ลาพักร้อน ในวันที่ 6 กันยายน 2021 ย้ายไปที่ 7 กันยายน 2021
+    1.9 กดปุ่ม My Leave และตรวจสอบข้อมูลของ Leave ID 3724</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1. พนักงานแก้ไขคำร้องการลาโดยการย้ายปุ่มไม่สำเร็จ
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   1.1 ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
+   1.2 ระบบจะแสดงหน้าจอสำหรับกรอกข้อมูลการลา (LEAVE004)
+   1.3 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
+เป็นข้อมูลที่ผู้ใช้เลือก
+   1.4 ระบบจะแสดงหน้าจอปฏิทิน (LEAVE005) ของเดือนสิงหาคม ค.ศ. 2021
+    1.5 แสดงปุ่มย่อยให้เลือก (drop down)
+    1.6 ระบบแสดงหน้าจอ (LEAVE008) เพื่อแสดงข้อมูลทั้งหมดของผู้ใช้ 
+    1.7 ตัวเลือกลากิจ/ลาพักร้อน ในวันที่ 7 กันยายน 2021 ไม่สามารถย้ายไปที่ 8 กันยายน 2021 ได้</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1. พนักงานแก้ไขคำร้องการลาโดยการย้ายปุ่มสำเร็จ
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   1.1 ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
+   1.2 ระบบจะแสดงหน้าจอสำหรับกรอกข้อมูลการลา (LEAVE004)
+   1.3 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
+เป็นข้อมูลที่ผู้ใช้เลือก
+   1.4 ระบบจะแสดงหน้าจอปฏิทิน (LEAVE005) ของเดือนสิงหาคม ค.ศ. 2021
+    1.1 แสดงปุ่มย่อยให้เลือก (drop down)
+    1.2 ระบบแสดงหน้าจอ (LEAVE008) เพื่อแสดงข้อมูลทั้งหมดของผู้ใช้ 
+    1.3 ตัวเลือกลากิจ/ลาพักร้อน ในวันที่ 7 กันยายน 2021 ไม่สามารถย้ายไปที่ 8 กันยายน 2021 ได้</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1. พนักงานแก้ไขคำร้องการลาโดยการย้ายปุ่มสำเร็จ
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   1.1 ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
+   1.2 ระบบจะแสดงหน้าจอสำหรับกรอกข้อมูลการลา (LEAVE004)
+   1.3 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004)
+เป็นข้อมูลที่ผู้ใช้เลือก
+   1.4 ระบบจะแสดงหน้าจอปฏิทิน (LEAVE005) ของเดือนสิงหาคม ค.ศ. 2021
+    1.5 แสดงปุ่มย่อยให้เลือก (drop down)
+    1.6 ระบบแสดงหน้าจอ (LEAVE008) เพื่อแสดงข้อมูลทั้งหมดของผู้ใช้ 
+    1.7 ระบบแสดงปฏิทินในเดือนกันยายน
+    1.8ตัวเลือกลากิจ/ลาพักร้อน ในวันที่ 7 กันยายน 2021 ย้ายไปที่ 8 กันยายน 2021 ได้
+    1.9 ระบบแสดงหน้าจอสำหรับข้อมูลการลา (LEAVE003) และข้อมูลมีการเปี่ยนแปลงดังนี้
+Leave ID : 3724, Submit Date : 25-08-2021 11:14
+The applicant : "test_it_role", Type of leave : "ลากิจ/ลาพักร้อน"
+Start date (Since) : 06-09-2021, End date (Until) : 07-09-2021
+Amount the day : 1.000, Status : "Waiting for approve"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1. พนักงานแก้ไขคำร้องการลาโดยการย้ายปุ่มไม่สำเร็จ
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="TH Sarabun New"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   1.1 ระบบจะแสดงหน้าจอสำหรับการลา (LEAVE003)
+   1.2 ระบบจะแสดงหน้าจอสำหรับกรอกข้อมูลการลา (LEAVE004)
+   1.3 ระบบจะแสดงหน้าจอแสดงผลข้อมูลผู้ใช้งาน (LEAVE004) เป็นข้อมูลที่ผู้ใช้เลือก
+   1.4 ระบบจะแสดงหน้าจอปฏิทิน (LEAVE005) ของเดือนสิงหาคม ค.ศ. 2021
+    1.1 แสดงปุ่มย่อยให้เลือก (drop down)
+    1.2 ระบบแสดงหน้าจอ (LEAVE008) เพื่อแสดงข้อมูลทั้งหมดของผู้ใช้ 
+    1.3 ตัวเลือกลากิจ/ลาพักร้อน ในวันที่ 7 กันยายน 2021 ไม่สามารถย้ายไปที่ 8 กันยายน 2021 ได้</t>
     </r>
   </si>
 </sst>
@@ -5356,7 +5424,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5405,6 +5473,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -5446,7 +5520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5522,10 +5596,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
@@ -7304,9 +7379,9 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.6"/>
@@ -7324,14 +7399,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A1" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="31"/>
+      <c r="A1" s="33" t="s">
+        <v>377</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1" s="33"/>
       <c r="E1" s="15" t="s">
         <v>10</v>
       </c>
@@ -7342,10 +7417,10 @@
         <v>11</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="15"/>
@@ -7379,10 +7454,10 @@
         <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.6">
@@ -7497,10 +7572,10 @@
         <v>43</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>18</v>
@@ -7528,19 +7603,19 @@
         <v>91</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="4" customFormat="1" ht="231" x14ac:dyDescent="0.3">
@@ -7563,10 +7638,10 @@
         <v>145</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="I9" s="18"/>
       <c r="J9" s="8"/>
@@ -7586,16 +7661,16 @@
         <v>138</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>146</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="I10" s="18"/>
       <c r="J10" s="8"/>
@@ -7615,16 +7690,16 @@
         <v>138</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>147</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="I11" s="18"/>
       <c r="J11" s="8"/>
@@ -7641,19 +7716,19 @@
         <v>34</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="I12" s="18"/>
       <c r="J12" s="8"/>
@@ -7673,16 +7748,16 @@
         <v>138</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="I13" s="18"/>
       <c r="J13" s="8"/>
@@ -7702,16 +7777,16 @@
         <v>138</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="I14" s="18"/>
       <c r="J14" s="8"/>
@@ -7731,23 +7806,23 @@
         <v>138</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I15" s="16"/>
       <c r="J15" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="252" x14ac:dyDescent="0.3">
@@ -7764,23 +7839,23 @@
         <v>138</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="I16" s="16"/>
       <c r="J16" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="4" customFormat="1" ht="273" x14ac:dyDescent="0.3">
@@ -7797,23 +7872,23 @@
         <v>138</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I17" s="16"/>
       <c r="J17" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="4" customFormat="1" ht="273" x14ac:dyDescent="0.3">
@@ -7830,21 +7905,21 @@
         <v>138</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="I18" s="16"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="4" customFormat="1" ht="168" x14ac:dyDescent="0.3">
@@ -7861,21 +7936,21 @@
         <v>138</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="I19" s="18"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="4" customFormat="1" ht="231" x14ac:dyDescent="0.3">
@@ -7892,21 +7967,21 @@
         <v>138</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I20" s="16"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="4" customFormat="1" ht="168" x14ac:dyDescent="0.3">
@@ -7923,21 +7998,21 @@
         <v>138</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I21" s="18"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="4" customFormat="1" ht="252" x14ac:dyDescent="0.3">
@@ -7954,16 +8029,16 @@
         <v>138</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="I22" s="18"/>
       <c r="J22" s="8"/>
@@ -7974,25 +8049,25 @@
         <v>57</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>138</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="I23" s="18"/>
       <c r="J23" s="8"/>
@@ -8012,16 +8087,16 @@
         <v>138</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>338</v>
+        <v>370</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>339</v>
+        <v>371</v>
       </c>
       <c r="I24" s="18"/>
       <c r="J24" s="8"/>
@@ -8043,7 +8118,7 @@
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" s="10" customFormat="1" ht="273" x14ac:dyDescent="0.3">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="12" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="13" t="s">
@@ -8056,21 +8131,21 @@
         <v>140</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="I26" s="18"/>
       <c r="J26" s="12"/>
       <c r="K26" s="21" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="10" customFormat="1" ht="273" x14ac:dyDescent="0.3">
@@ -8087,16 +8162,16 @@
         <v>141</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="I27" s="18"/>
       <c r="J27" s="12"/>
@@ -8116,16 +8191,16 @@
         <v>142</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="I28" s="18"/>
       <c r="J28" s="12"/>
@@ -8145,16 +8220,16 @@
         <v>143</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="I29" s="18"/>
       <c r="J29" s="12"/>
@@ -8165,25 +8240,25 @@
         <v>93</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>154</v>
+        <v>368</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>122</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>371</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>158</v>
+        <v>375</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>369</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>343</v>
+        <v>373</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>344</v>
+        <v>374</v>
       </c>
       <c r="I30" s="18"/>
       <c r="J30" s="12"/>
@@ -8203,23 +8278,23 @@
         <v>143</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="I31" s="18"/>
       <c r="J31" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="K31" s="12" t="s">
         <v>201</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="10" customFormat="1" ht="189" x14ac:dyDescent="0.3">
@@ -8236,20 +8311,20 @@
         <v>143</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="F32" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="G32" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="G32" s="13" t="s">
-        <v>212</v>
-      </c>
       <c r="H32" s="13" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="I32" s="16"/>
       <c r="K32" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="10" customFormat="1" ht="294" x14ac:dyDescent="0.3">
@@ -8266,23 +8341,23 @@
         <v>144</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="I33" s="18"/>
       <c r="J33" s="12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K33" s="12" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="10" customFormat="1" ht="210" x14ac:dyDescent="0.3">
@@ -8299,78 +8374,78 @@
         <v>144</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="F34" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="H34" s="13" t="s">
         <v>216</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>218</v>
       </c>
       <c r="I34" s="16"/>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
     </row>
-    <row r="35" spans="1:11" s="10" customFormat="1" ht="210" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" s="10" customFormat="1" ht="315" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="13" t="s">
         <v>131</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>133</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>159</v>
+        <v>378</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>380</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>219</v>
+        <v>381</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>223</v>
+        <v>384</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>222</v>
+        <v>383</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="12" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="K35" s="12" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="10" customFormat="1" ht="84" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" s="10" customFormat="1" ht="210" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="13" t="s">
         <v>132</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>133</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>159</v>
+        <v>378</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>380</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>221</v>
+        <v>379</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>224</v>
+        <v>382</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>224</v>
+        <v>385</v>
       </c>
       <c r="I36" s="18"/>
       <c r="J36" s="12"/>
@@ -8392,7 +8467,7 @@
       <c r="K37" s="6"/>
     </row>
     <row r="38" spans="1:11" s="10" customFormat="1" ht="126" x14ac:dyDescent="0.3">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="31" t="s">
         <v>100</v>
       </c>
       <c r="B38" s="13" t="s">
@@ -8402,26 +8477,26 @@
         <v>125</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="I38" s="18"/>
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
     </row>
     <row r="39" spans="1:11" s="10" customFormat="1" ht="147" x14ac:dyDescent="0.3">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="31" t="s">
         <v>101</v>
       </c>
       <c r="B39" s="13" t="s">
@@ -8431,26 +8506,26 @@
         <v>125</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I39" s="18"/>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
     </row>
     <row r="40" spans="1:11" s="10" customFormat="1" ht="147" x14ac:dyDescent="0.3">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="31" t="s">
         <v>102</v>
       </c>
       <c r="B40" s="13" t="s">
@@ -8460,26 +8535,26 @@
         <v>125</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="I40" s="18"/>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
     </row>
     <row r="41" spans="1:11" s="10" customFormat="1" ht="84" x14ac:dyDescent="0.3">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="31" t="s">
         <v>103</v>
       </c>
       <c r="B41" s="13" t="s">
@@ -8489,19 +8564,19 @@
         <v>125</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="I41" s="18"/>
       <c r="J41" s="12"/>
@@ -8523,7 +8598,7 @@
       <c r="K42" s="6"/>
     </row>
     <row r="43" spans="1:11" s="4" customFormat="1" ht="294" x14ac:dyDescent="0.3">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="31" t="s">
         <v>104</v>
       </c>
       <c r="B43" s="13" t="s">
@@ -8536,27 +8611,27 @@
         <v>139</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="I43" s="16"/>
       <c r="J43" s="8" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="4" customFormat="1" ht="168" x14ac:dyDescent="0.3">
-      <c r="A44" s="12" t="s">
+      <c r="A44" s="31" t="s">
         <v>105</v>
       </c>
       <c r="B44" s="13" t="s">
@@ -8569,27 +8644,27 @@
         <v>139</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="I44" s="16"/>
       <c r="J44" s="8" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.3">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="31" t="s">
         <v>106</v>
       </c>
       <c r="B45" s="13" t="s">
@@ -8602,27 +8677,27 @@
         <v>139</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="I45" s="16"/>
       <c r="J45" s="8" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="409.6" x14ac:dyDescent="0.6">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="31" t="s">
         <v>107</v>
       </c>
       <c r="B46" s="13" t="s">
@@ -8635,27 +8710,27 @@
         <v>139</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="I46" s="16"/>
       <c r="J46" s="8" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="105" x14ac:dyDescent="0.6">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="31" t="s">
         <v>108</v>
       </c>
       <c r="B47" s="13" t="s">
@@ -8668,27 +8743,27 @@
         <v>139</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="H47" s="13" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="I47" s="16"/>
       <c r="J47" s="8" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="168" x14ac:dyDescent="0.6">
-      <c r="A48" s="12" t="s">
+      <c r="A48" s="31" t="s">
         <v>109</v>
       </c>
       <c r="B48" s="13" t="s">
@@ -8701,27 +8776,27 @@
         <v>139</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="I48" s="16"/>
       <c r="J48" s="8" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="105" x14ac:dyDescent="0.6">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="31" t="s">
         <v>110</v>
       </c>
       <c r="B49" s="13" t="s">
@@ -8734,23 +8809,23 @@
         <v>139</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="I49" s="16"/>
       <c r="J49" s="8" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.6">
@@ -8769,7 +8844,7 @@
       <c r="K50" s="5"/>
     </row>
     <row r="51" spans="1:12" ht="273" x14ac:dyDescent="0.6">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="31" t="s">
         <v>111</v>
       </c>
       <c r="B51" s="12" t="s">
@@ -8779,30 +8854,30 @@
         <v>137</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F51" s="23" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="G51" s="23" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="H51" s="23" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="I51" s="24"/>
       <c r="J51" s="8" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="273" x14ac:dyDescent="0.6">
-      <c r="A52" s="12" t="s">
+      <c r="A52" s="31" t="s">
         <v>112</v>
       </c>
       <c r="B52" s="12" t="s">
@@ -8812,19 +8887,19 @@
         <v>137</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F52" s="23" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="G52" s="23" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="H52" s="23" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="I52" s="25"/>
       <c r="J52" s="11"/>
@@ -8832,7 +8907,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A53" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -8846,186 +8921,186 @@
       <c r="K53" s="5"/>
     </row>
     <row r="54" spans="1:12" ht="126" x14ac:dyDescent="0.6">
-      <c r="A54" s="12" t="s">
+      <c r="A54" s="31" t="s">
         <v>113</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="G54" s="20" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="H54" s="20" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="I54" s="18"/>
       <c r="J54" s="11"/>
       <c r="K54" s="11"/>
     </row>
     <row r="55" spans="1:12" ht="105" x14ac:dyDescent="0.6">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="31" t="s">
         <v>114</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E55" s="14" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="G55" s="20" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="H55" s="20" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="I55" s="18"/>
       <c r="J55" s="11"/>
       <c r="K55" s="11"/>
     </row>
     <row r="56" spans="1:12" ht="126" x14ac:dyDescent="0.6">
-      <c r="A56" s="12" t="s">
+      <c r="A56" s="31" t="s">
         <v>115</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="G56" s="20" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="H56" s="20" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="I56" s="16"/>
       <c r="J56" s="8" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="K56" s="7" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="126" x14ac:dyDescent="0.6">
-      <c r="A57" s="12" t="s">
+      <c r="A57" s="31" t="s">
         <v>116</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C57" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="D57" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="D57" s="13" t="s">
-        <v>179</v>
-      </c>
       <c r="E57" s="14" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G57" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="H57" s="20" t="s">
         <v>300</v>
-      </c>
-      <c r="H57" s="20" t="s">
-        <v>307</v>
       </c>
       <c r="I57" s="16"/>
       <c r="J57" s="8" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="K57" s="7" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="126" x14ac:dyDescent="0.6">
-      <c r="A58" s="12" t="s">
+      <c r="A58" s="31" t="s">
         <v>117</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E58" s="14" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="G58" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="H58" s="20" t="s">
         <v>301</v>
-      </c>
-      <c r="H58" s="20" t="s">
-        <v>308</v>
       </c>
       <c r="I58" s="16"/>
       <c r="J58" s="8" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="K58" s="8" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="84" x14ac:dyDescent="0.6">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="31" t="s">
         <v>120</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G59" s="20" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="H59" s="20" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="I59" s="18"/>
       <c r="J59" s="8"/>
@@ -9033,7 +9108,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A60" s="5" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -9047,42 +9122,42 @@
       <c r="K60" s="5"/>
     </row>
     <row r="61" spans="1:12" ht="126" x14ac:dyDescent="0.6">
-      <c r="A61" s="12" t="s">
+      <c r="A61" s="31" t="s">
         <v>121</v>
       </c>
       <c r="B61" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="H61" s="7" t="s">
         <v>312</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="F61" s="14" t="s">
-        <v>315</v>
-      </c>
-      <c r="G61" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="H61" s="7" t="s">
-        <v>319</v>
       </c>
       <c r="I61" s="16"/>
       <c r="J61" s="8" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="K61" s="8" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="L61" s="4"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A62" s="6" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -9101,13 +9176,13 @@
         <v>126</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="C63" s="27" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="D63" s="27" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="E63" s="26"/>
       <c r="F63" s="26"/>
@@ -9269,14 +9344,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.6">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="32"/>
       <c r="E1" s="15" t="s">
         <v>10</v>
       </c>
@@ -9287,10 +9362,10 @@
         <v>11</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="15"/>
@@ -9324,10 +9399,10 @@
         <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.6">
@@ -9359,7 +9434,7 @@
         <v>42</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>20</v>
@@ -9390,7 +9465,7 @@
         <v>42</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>23</v>
@@ -9442,10 +9517,10 @@
         <v>43</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>18</v>

</xml_diff>